<commit_message>
Added "Drop in power" to the RSSI-dBm spreadsheet
</commit_message>
<xml_diff>
--- a/docs/RSSI-Percentage.xlsx
+++ b/docs/RSSI-Percentage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richb/github/wifi-heatmapper/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F5AD1E-79E2-E64E-9311-45AF1DF0160F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE95A4BB-513F-E646-9516-64B63D9AE959}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4600" yWindow="2220" windowWidth="23500" windowHeight="11680" xr2:uid="{87C5B918-C82E-5544-BD36-195150776B85}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Percentage</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Percent</t>
   </si>
   <si>
-    <t>dBm/dBm</t>
-  </si>
-  <si>
     <t>Changes</t>
   </si>
   <si>
@@ -72,12 +69,25 @@
   </si>
   <si>
     <t>interpolation</t>
+  </si>
+  <si>
+    <t>drop in power</t>
+  </si>
+  <si>
+    <t>from -40dBm</t>
+  </si>
+  <si>
+    <t>Added "Drop in power" column (pink) to show how weak signal gets when dBm's drop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.000000%"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -87,7 +97,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +107,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,12 +141,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,21 +485,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7367EF-27CB-9D45-A2A7-00F895A954E9}">
-  <dimension ref="A2:H19"/>
+  <dimension ref="A2:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="1.83203125" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="1.5" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="2"/>
+    <col min="10" max="10" width="1.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" style="9" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -455,335 +512,644 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M3" s="12"/>
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5">
+      <c r="J5" s="15"/>
+      <c r="K5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
-        <f>(B5/100)*60-100</f>
+      <c r="L5" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f>(B6/100)*60-100</f>
         <v>-100</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>-100</v>
       </c>
-      <c r="F5" s="2">
-        <f>(E5+100)/60</f>
+      <c r="F6" s="2">
+        <f>(E6+100)/60</f>
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G6" s="2"/>
+      <c r="H6">
         <v>-100</v>
       </c>
-      <c r="H5" s="2">
-        <f>(G5+100)/60</f>
+      <c r="I6" s="2">
+        <f>(H6+100)/60</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6">
+      <c r="K6" s="2">
+        <f>(L6+100)/60</f>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>-40</v>
+      </c>
+      <c r="M6" s="9">
+        <f>50%^(($L$6-L6)/3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B7">
         <v>10</v>
       </c>
-      <c r="C6">
-        <f t="shared" ref="C6:C17" si="0">(B6/100)*60-100</f>
+      <c r="C7">
+        <f t="shared" ref="C7:C18" si="0">(B7/100)*60-100</f>
         <v>-94</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>-94</v>
       </c>
-      <c r="F6" s="2">
-        <f t="shared" ref="F6:F17" si="1">(E6+100)/60</f>
+      <c r="F7" s="2">
+        <f t="shared" ref="F7:F18" si="1">(E7+100)/60</f>
         <v>0.1</v>
       </c>
-      <c r="G6">
+      <c r="G7" s="2"/>
+      <c r="H7">
         <v>-90</v>
       </c>
-      <c r="H6" s="2">
-        <f t="shared" ref="H6:H15" si="2">(G6+100)/60</f>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I16" si="2">(H7+100)/60</f>
         <v>0.16666666666666666</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7">
+      <c r="K7" s="2">
+        <f t="shared" ref="K7:K26" si="3">(L7+100)/60</f>
+        <v>0.95</v>
+      </c>
+      <c r="L7">
+        <f>L6-3</f>
+        <v>-43</v>
+      </c>
+      <c r="M7" s="9">
+        <f t="shared" ref="M7:M26" si="4">50%^(($L$6-L7)/3)</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B8">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>-88</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>-88</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F8" s="2">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="G7">
+      <c r="G8" s="2"/>
+      <c r="H8">
         <v>-80</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I8" s="2">
         <f t="shared" si="2"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8">
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ref="L8:L26" si="5">L7-3</f>
+        <v>-46</v>
+      </c>
+      <c r="M8" s="9">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B9">
         <v>25</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <f t="shared" si="0"/>
         <v>-85</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>-85</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="G8">
+      <c r="G9" s="2"/>
+      <c r="H9">
         <v>-75</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I9" s="2">
         <f t="shared" si="2"/>
         <v>0.41666666666666669</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9">
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>0.85</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="5"/>
+        <v>-49</v>
+      </c>
+      <c r="M9" s="9">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B10">
         <v>30</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>-82</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>-82</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F10" s="2">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="G9">
+      <c r="G10" s="2"/>
+      <c r="H10">
         <v>-70</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I10" s="2">
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10">
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="5"/>
+        <v>-52</v>
+      </c>
+      <c r="M10" s="9">
+        <f t="shared" si="4"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B11">
         <v>40</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <f t="shared" si="0"/>
         <v>-76</v>
       </c>
-      <c r="E10">
+      <c r="E11">
         <v>-76</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="G10">
+      <c r="G11" s="2"/>
+      <c r="H11">
         <v>-65</v>
       </c>
-      <c r="H10" s="2">
+      <c r="I11" s="2">
         <f t="shared" si="2"/>
         <v>0.58333333333333337</v>
       </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11">
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.75</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="5"/>
+        <v>-55</v>
+      </c>
+      <c r="M11" s="9">
+        <f t="shared" si="4"/>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B12">
         <v>50</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <f t="shared" si="0"/>
         <v>-70</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>-70</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F12" s="2">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="G11">
+      <c r="G12" s="2"/>
+      <c r="H12">
         <v>-60</v>
       </c>
-      <c r="H11" s="2">
+      <c r="I12" s="2">
         <f t="shared" si="2"/>
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12">
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="5"/>
+        <v>-58</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" si="4"/>
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B13">
         <v>60</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <f t="shared" si="0"/>
         <v>-64</v>
       </c>
-      <c r="E12">
+      <c r="E13">
         <v>-64</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F13" s="2">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="G12">
+      <c r="G13" s="2"/>
+      <c r="H13">
         <v>-55</v>
       </c>
-      <c r="H12" s="2">
+      <c r="I13" s="2">
         <f t="shared" si="2"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13">
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.65</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="5"/>
+        <v>-61</v>
+      </c>
+      <c r="M13" s="9">
+        <f t="shared" si="4"/>
+        <v>7.8125E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B14">
         <v>70</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <f t="shared" si="0"/>
         <v>-58</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>-58</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="2">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="G13">
+      <c r="G14" s="2"/>
+      <c r="H14">
         <v>-50</v>
       </c>
-      <c r="H13" s="2">
+      <c r="I14" s="2">
         <f t="shared" si="2"/>
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14">
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="5"/>
+        <v>-64</v>
+      </c>
+      <c r="M14" s="9">
+        <f t="shared" si="4"/>
+        <v>3.90625E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B15">
         <v>75</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <f t="shared" si="0"/>
         <v>-55</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>-55</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F15" s="2">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
-      <c r="G14">
+      <c r="G15" s="2"/>
+      <c r="H15">
         <v>-45</v>
       </c>
-      <c r="H14" s="2">
+      <c r="I15" s="2">
         <f t="shared" si="2"/>
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15">
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="5"/>
+        <v>-67</v>
+      </c>
+      <c r="M15" s="9">
+        <f t="shared" si="4"/>
+        <v>1.953125E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B16">
         <v>80</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <f t="shared" si="0"/>
         <v>-52</v>
       </c>
-      <c r="E15">
+      <c r="E16">
         <v>-52</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F16" s="2">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="G15">
+      <c r="G16" s="2"/>
+      <c r="H16">
         <v>-40</v>
       </c>
-      <c r="H15" s="2">
+      <c r="I16" s="2">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16">
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="5"/>
+        <v>-70</v>
+      </c>
+      <c r="M16" s="9">
+        <f t="shared" si="4"/>
+        <v>9.765625E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B17">
         <v>90</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <f t="shared" si="0"/>
         <v>-46</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>-46</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="2">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B17">
+      <c r="G17" s="2"/>
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>0.45</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="5"/>
+        <v>-73</v>
+      </c>
+      <c r="M17" s="9">
+        <f t="shared" si="4"/>
+        <v>4.8828125E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B18">
         <v>100</v>
       </c>
-      <c r="C17">
+      <c r="C18">
         <f t="shared" si="0"/>
         <v>-40</v>
       </c>
-      <c r="E17">
+      <c r="E18">
         <v>-40</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="2"/>
+      <c r="K18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="5"/>
+        <v>-76</v>
+      </c>
+      <c r="M18" s="9">
+        <f t="shared" si="4"/>
+        <v>2.44140625E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>0.35</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>-79</v>
+      </c>
+      <c r="M19" s="9">
+        <f t="shared" si="4"/>
+        <v>1.220703125E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
         <v>45</v>
       </c>
-      <c r="C19">
-        <f t="shared" ref="C19" si="3">(B19/100)*60-100</f>
+      <c r="C20">
+        <f t="shared" ref="C20" si="6">(B20/100)*60-100</f>
         <v>-73</v>
       </c>
-      <c r="E19">
+      <c r="E20">
         <v>-56</v>
       </c>
-      <c r="F19" s="2">
-        <f t="shared" ref="F19" si="4">(E19+100)/60</f>
+      <c r="F20" s="2">
+        <f t="shared" ref="F20" si="7">(E20+100)/60</f>
         <v>0.73333333333333328</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="K20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="5"/>
+        <v>-82</v>
+      </c>
+      <c r="M20" s="9">
+        <f t="shared" si="4"/>
+        <v>6.103515625E-5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="5"/>
+        <v>-85</v>
+      </c>
+      <c r="M21" s="9">
+        <f t="shared" si="4"/>
+        <v>3.0517578125E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.2</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="5"/>
+        <v>-88</v>
+      </c>
+      <c r="M22" s="9">
+        <f t="shared" si="4"/>
+        <v>1.52587890625E-5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="5"/>
+        <v>-91</v>
+      </c>
+      <c r="M23" s="9">
+        <f t="shared" si="4"/>
+        <v>7.62939453125E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="5"/>
+        <v>-94</v>
+      </c>
+      <c r="M24" s="9">
+        <f t="shared" si="4"/>
+        <v>3.814697265625E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K25" s="2">
+        <f t="shared" si="3"/>
+        <v>0.05</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="5"/>
+        <v>-97</v>
+      </c>
+      <c r="M25" s="9">
+        <f t="shared" si="4"/>
+        <v>1.9073486328125E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K26" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="5"/>
+        <v>-100</v>
+      </c>
+      <c r="M26" s="9">
+        <f t="shared" si="4"/>
+        <v>9.5367431640625E-7</v>
       </c>
     </row>
   </sheetData>
@@ -794,17 +1160,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA8F60B-A847-4849-B571-FF8ACE644846}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -812,7 +1178,7 @@
         <v>45717</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -820,17 +1186,25 @@
         <v>45904</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>45907</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>